<commit_message>
Added a server so that the bot will run continuously
</commit_message>
<xml_diff>
--- a/Assignments.xlsx
+++ b/Assignments.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucd-my.sharepoint.com/personal/michael_davitt_ucdconnect_ie/Documents/Documents/Projects/Assignments_Bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{72B1BF19-CFB7-45A9-BC12-ACA135719C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:40009_{72B1BF19-CFB7-45A9-BC12-ACA135719C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7D8F9931-C0F9-4749-9E4E-B010BE2C68FF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignments" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="37">
   <si>
     <t>Assignment</t>
   </si>
@@ -79,15 +79,9 @@
     <t>Week 13</t>
   </si>
   <si>
-    <t>Practicals</t>
-  </si>
-  <si>
     <t>Java Programming</t>
   </si>
   <si>
-    <t>Ongoing (4 total)</t>
-  </si>
-  <si>
     <t>Programming Project</t>
   </si>
   <si>
@@ -125,12 +119,24 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>Practical 2</t>
+  </si>
+  <si>
+    <t>Practical 3</t>
+  </si>
+  <si>
+    <t>Practical 5</t>
+  </si>
+  <si>
+    <t>Practical 7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -966,11 +972,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,7 +1037,7 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D4" s="2">
         <v>0.4</v>
@@ -1081,155 +1087,197 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>21</v>
+      <c r="C10" s="1">
+        <v>44238</v>
       </c>
       <c r="D10" s="2">
-        <v>0.3</v>
+        <v>7.4999999999999997E-2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" t="s">
-        <v>34</v>
+        <v>19</v>
+      </c>
+      <c r="C11" s="1">
+        <v>44610</v>
       </c>
       <c r="D11" s="2">
-        <v>0.3</v>
+        <v>7.4999999999999997E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" t="s">
-        <v>34</v>
+        <v>19</v>
+      </c>
+      <c r="C12" s="1">
+        <v>44624</v>
       </c>
       <c r="D12" s="2">
-        <v>0.4</v>
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="1">
+        <v>44638</v>
+      </c>
+      <c r="D13" s="2">
+        <v>7.4999999999999997E-2</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="D14" s="2">
-        <v>0.85</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="1">
-        <v>44598</v>
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
       </c>
       <c r="D15" s="2">
-        <v>0.15</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D17" s="2">
-        <v>0.6</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" t="s">
-        <v>34</v>
+        <v>2</v>
+      </c>
+      <c r="C18" s="1">
+        <v>44598</v>
       </c>
       <c r="D18" s="2">
-        <v>0.4</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D20" s="2">
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D21" s="2">
         <v>0.4</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="2">
-        <v>0.2</v>
-      </c>
-    </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>30</v>
       </c>
-      <c r="C23" t="s">
-        <v>34</v>
-      </c>
-      <c r="D23" s="2">
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="2">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sorted the output by days until due and fixed small type in xlsx file
</commit_message>
<xml_diff>
--- a/Assignments.xlsx
+++ b/Assignments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucd-my.sharepoint.com/personal/michael_davitt_ucdconnect_ie/Documents/Documents/Projects/Assignments_Bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:40009_{72B1BF19-CFB7-45A9-BC12-ACA135719C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7D8F9931-C0F9-4749-9E4E-B010BE2C68FF}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:40009_{72B1BF19-CFB7-45A9-BC12-ACA135719C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6E57C07-4CE8-43E8-AA76-03544BB308EA}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -976,7 +976,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1093,7 +1093,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="1">
-        <v>44238</v>
+        <v>44603</v>
       </c>
       <c r="D10" s="2">
         <v>7.4999999999999997E-2</v>

</xml_diff>

<commit_message>
Updated assignments file with new dates, fixed timestamp issue, and split the final message when it was too long
</commit_message>
<xml_diff>
--- a/Assignments.xlsx
+++ b/Assignments.xlsx
@@ -8,19 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucd-my.sharepoint.com/personal/michael_davitt_ucdconnect_ie/Documents/Documents/Projects/Assignments_Bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:40009_{72B1BF19-CFB7-45A9-BC12-ACA135719C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6E57C07-4CE8-43E8-AA76-03544BB308EA}"/>
+  <xr:revisionPtr revIDLastSave="104" documentId="13_ncr:40009_{72B1BF19-CFB7-45A9-BC12-ACA135719C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E461BD52-2E20-4715-986F-FC9C7A4CC8DF}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignments" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="39">
   <si>
     <t>Assignment</t>
   </si>
@@ -46,39 +57,21 @@
     <t>Networks and Internet Systems</t>
   </si>
   <si>
-    <t>week 6</t>
-  </si>
-  <si>
     <t>Practical Test</t>
   </si>
   <si>
-    <t>Week 12</t>
-  </si>
-  <si>
     <t>End of Trimester Exam</t>
   </si>
   <si>
-    <t>Practical Sessions</t>
-  </si>
-  <si>
-    <t>Ongoing</t>
-  </si>
-  <si>
     <t>Data Understanding and Prep</t>
   </si>
   <si>
     <t>Data Analytics</t>
   </si>
   <si>
-    <t>week 7</t>
-  </si>
-  <si>
     <t>Model Selection and Evaluation</t>
   </si>
   <si>
-    <t>Week 13</t>
-  </si>
-  <si>
     <t>Java Programming</t>
   </si>
   <si>
@@ -88,9 +81,6 @@
     <t>In Class Test</t>
   </si>
   <si>
-    <t>week 11</t>
-  </si>
-  <si>
     <t>Software Requirement Specification</t>
   </si>
   <si>
@@ -131,6 +121,33 @@
   </si>
   <si>
     <t>Practical 7</t>
+  </si>
+  <si>
+    <t>Week 3 Practical</t>
+  </si>
+  <si>
+    <t>Week 4 Practical</t>
+  </si>
+  <si>
+    <t>Week 5 Practical</t>
+  </si>
+  <si>
+    <t>Week 6 Practical</t>
+  </si>
+  <si>
+    <t>Week 7 Practical</t>
+  </si>
+  <si>
+    <t>Week 8 Practical</t>
+  </si>
+  <si>
+    <t>Week 9 Practical</t>
+  </si>
+  <si>
+    <t>Week 10 Practical</t>
+  </si>
+  <si>
+    <t>Week 11 Practical</t>
   </si>
 </sst>
 </file>
@@ -454,7 +471,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -569,6 +586,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -614,10 +646,29 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -973,311 +1024,460 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="6">
+        <v>44613</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2">
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="6">
+        <v>44670</v>
+      </c>
+      <c r="D3" s="3">
         <v>0.2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" s="6">
+        <v>44691</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="6">
+        <v>44594</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="6">
+        <v>44601</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="6">
+        <v>44608</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="6">
+        <v>44615</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="6">
+        <v>44622</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="6">
+        <v>44643</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="6">
+        <v>44650</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="6">
+        <v>44657</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="6">
+        <v>44664</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="2">
+      <c r="B16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="6">
+        <v>44624</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="6">
+        <v>44666</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="6">
+        <v>44603</v>
+      </c>
+      <c r="D19" s="3">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="6">
+        <v>44610</v>
+      </c>
+      <c r="D20" s="3">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="6">
+        <v>44624</v>
+      </c>
+      <c r="D21" s="3">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="6">
+        <v>44638</v>
+      </c>
+      <c r="D22" s="3">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="6">
+        <v>44652</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="6">
+        <v>44669</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="6">
+        <v>44666</v>
+      </c>
+      <c r="D26" s="3">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="6">
+        <v>44598</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" s="6">
+        <v>44680</v>
+      </c>
+      <c r="D30" s="3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33" s="3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D34" s="3">
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="1">
-        <v>44603</v>
-      </c>
-      <c r="D10" s="2">
-        <v>7.4999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="1">
-        <v>44610</v>
-      </c>
-      <c r="D11" s="2">
-        <v>7.4999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="1">
-        <v>44624</v>
-      </c>
-      <c r="D12" s="2">
-        <v>7.4999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="1">
-        <v>44638</v>
-      </c>
-      <c r="D13" s="2">
-        <v>7.4999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="2">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="2">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="2">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="1">
-        <v>44598</v>
-      </c>
-      <c r="D18" s="2">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="C35" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C20" t="s">
-        <v>32</v>
-      </c>
-      <c r="D20" s="2">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="2">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="2">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" t="s">
-        <v>32</v>
-      </c>
-      <c r="D24" s="2">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" t="s">
-        <v>32</v>
-      </c>
-      <c r="D25" s="2">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" t="s">
-        <v>32</v>
-      </c>
-      <c r="D26" s="2">
+      <c r="D35" s="3">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>